<commit_message>
Contact us Prod changes
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC32_Verify_store_location.xlsx
+++ b/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC32_Verify_store_location.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\Prod\ALL_PAGES\END_TO_END\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Actual_testcases\Kaman\Prod\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16246D0-E435-46DD-8B1E-7BB23CB774DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B1F911-C80D-4ADE-9EB4-24D9997F19E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
   <si>
     <t>TestCase</t>
   </si>
@@ -74,21 +74,9 @@
     <t>ContactMenu</t>
   </si>
   <si>
-    <t>VERIFY_TEXT_PRESENT</t>
-  </si>
-  <si>
-    <t>Storelocator</t>
-  </si>
-  <si>
     <t>ContactList</t>
   </si>
   <si>
-    <t>StorelocatorZip</t>
-  </si>
-  <si>
-    <t>StorelocatorSearchButton</t>
-  </si>
-  <si>
     <t>zip</t>
   </si>
   <si>
@@ -123,6 +111,42 @@
   </si>
   <si>
     <t>$Registered_Password</t>
+  </si>
+  <si>
+    <t>ContactUSHeader</t>
+  </si>
+  <si>
+    <t>ContactUsMessage</t>
+  </si>
+  <si>
+    <t>WAIT</t>
+  </si>
+  <si>
+    <t>This is test message</t>
+  </si>
+  <si>
+    <t>ContactUsDropdown</t>
+  </si>
+  <si>
+    <t>DROPDOWN_SELECT</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>SendContactusDetails</t>
+  </si>
+  <si>
+    <t>ContactUsConfirmation</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>XYZ Corp</t>
+  </si>
+  <si>
+    <t>TINY_SCROLL_DOWN</t>
   </si>
 </sst>
 </file>
@@ -539,17 +563,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" customWidth="1"/>
   </cols>
@@ -587,13 +611,13 @@
     <row r="3" spans="1:5">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E3" s="5"/>
     </row>
@@ -603,10 +627,10 @@
         <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E4" s="5"/>
     </row>
@@ -619,7 +643,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
@@ -634,7 +658,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>15</v>
@@ -646,40 +670,33 @@
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="3"/>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3"/>
       <c r="B9" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3"/>
@@ -687,13 +704,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -702,57 +719,53 @@
         <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3"/>
       <c r="B12" s="5" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3"/>
       <c r="B13" s="5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3"/>
-      <c r="B14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="B14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3"/>
@@ -760,25 +773,53 @@
         <v>11</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3"/>
       <c r="B16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3"/>
+      <c r="B17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3"/>
+      <c r="B18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -789,15 +830,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection activeCell="A12" sqref="A12:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -814,7 +855,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -822,7 +863,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -830,12 +871,12 @@
         <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="5" t="b">
         <v>1</v>
@@ -843,7 +884,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B6" s="5" t="b">
         <v>1</v>
@@ -851,18 +892,50 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3">
         <v>10010</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>23</v>
+      <c r="A8" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -880,6 +953,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -1076,12 +1155,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>
@@ -1091,6 +1164,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1107,13 +1189,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>